<commit_message>
Cambio del archivo de excel para igualar a el archivo en drive.
</commit_message>
<xml_diff>
--- a/Equipo 2 - Requerimientos nuevos y Lista de Materiales - 2020B.xlsx
+++ b/Equipo 2 - Requerimientos nuevos y Lista de Materiales - 2020B.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Documents\Equipo2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55431C52-3387-4695-A220-0DCF13C9D12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C336BA3-7621-4517-B080-E6D91DC7F812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="149">
   <si>
     <t>Equipo #</t>
   </si>
@@ -269,12 +269,6 @@
   </si>
   <si>
     <t>WINDOW_LED10</t>
-  </si>
-  <si>
-    <t>PTE16</t>
-  </si>
-  <si>
-    <t>J5-02</t>
   </si>
   <si>
     <t>Entrada puenteada del último LED (LED10) de la barra de LEDs</t>
@@ -572,6 +566,18 @@
       <t xml:space="preserve"> when UNLOCK_BTN of the DCU transitions from BTN_NOT_PRESSED to BTN_PRESSED. After that, Driver Door shall set DCU_2.LockingReq back to 0x00 (NO_LOCKING_REQ) and keep it like this as long as there is no lock/unlock request from LOCK_BTN/UNLOCK_BTN.</t>
     </r>
   </si>
+  <si>
+    <t>PTA16</t>
+  </si>
+  <si>
+    <t>J5-03</t>
+  </si>
+  <si>
+    <t>PTB17</t>
+  </si>
+  <si>
+    <t>J4-06</t>
+  </si>
 </sst>
 </file>
 
@@ -648,7 +654,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -780,32 +786,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -1071,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1106,13 +1086,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1121,106 +1101,104 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1517,11 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
-      <selection activeCell="W45" sqref="W45"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1617,10 +1594,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="54"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1652,17 +1629,17 @@
       <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="52" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>17</v>
       </c>
       <c r="J4" s="3"/>
@@ -1684,29 +1661,29 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <v>12</v>
       </c>
       <c r="J5" s="3"/>
@@ -1728,29 +1705,29 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="21">
         <v>1</v>
       </c>
       <c r="J6" s="3"/>
@@ -1772,22 +1749,22 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="24" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="3"/>
@@ -1812,22 +1789,22 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="3"/>
@@ -1852,22 +1829,22 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="3"/>
@@ -1892,22 +1869,22 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="24" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="3"/>
@@ -1932,22 +1909,22 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="24" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="3"/>
@@ -1972,22 +1949,22 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="24" t="s">
         <v>43</v>
       </c>
       <c r="G12" s="3"/>
@@ -2011,23 +1988,23 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>48</v>
       </c>
       <c r="G13" s="3"/>
@@ -2051,23 +2028,23 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="54" t="s">
         <v>54</v>
       </c>
       <c r="G14" s="3"/>
@@ -2091,23 +2068,23 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="54" t="s">
         <v>57</v>
       </c>
       <c r="G15" s="3"/>
@@ -2131,23 +2108,23 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="54" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="3"/>
@@ -2171,23 +2148,23 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="54" t="s">
         <v>63</v>
       </c>
       <c r="G17" s="3"/>
@@ -2211,23 +2188,23 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="54" t="s">
         <v>66</v>
       </c>
       <c r="G18" s="3"/>
@@ -2251,23 +2228,23 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="54" t="s">
         <v>69</v>
       </c>
       <c r="G19" s="3"/>
@@ -2291,23 +2268,23 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="54" t="s">
         <v>72</v>
       </c>
       <c r="G20" s="3"/>
@@ -2331,23 +2308,23 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="54" t="s">
         <v>75</v>
       </c>
       <c r="G21" s="3"/>
@@ -2371,23 +2348,23 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="54" t="s">
         <v>78</v>
       </c>
       <c r="G22" s="3"/>
@@ -2411,24 +2388,24 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="29" t="s">
-        <v>80</v>
+      <c r="E23" s="53" t="s">
+        <v>145</v>
       </c>
-      <c r="F23" s="30" t="s">
-        <v>81</v>
+      <c r="F23" s="54" t="s">
+        <v>146</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2452,23 +2429,23 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="F24" s="54" t="s">
         <v>83</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>85</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2492,23 +2469,23 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="18" t="s">
+      <c r="F25" s="54" t="s">
         <v>87</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>89</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2532,23 +2509,23 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="F26" s="24" t="s">
         <v>91</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>93</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -2572,23 +2549,23 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>90</v>
+      <c r="C27" s="15" t="s">
+        <v>88</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>94</v>
+      <c r="D27" s="22" t="s">
+        <v>92</v>
       </c>
-      <c r="E27" s="25" t="s">
-        <v>22</v>
+      <c r="E27" s="23" t="s">
+        <v>147</v>
       </c>
-      <c r="F27" s="26" t="s">
-        <v>39</v>
+      <c r="F27" s="24" t="s">
+        <v>148</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2612,23 +2589,23 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="17" t="s">
+      <c r="E28" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="F28" s="56" t="s">
         <v>97</v>
-      </c>
-      <c r="E28" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>99</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -2652,23 +2629,23 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="F29" s="56" t="s">
         <v>101</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>103</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2691,24 +2668,24 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="18" t="s">
+      <c r="F30" s="54" t="s">
         <v>105</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>107</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2731,24 +2708,24 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="18" t="s">
+      <c r="F31" s="54" t="s">
         <v>109</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>111</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2772,23 +2749,23 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="F32" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>115</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2812,21 +2789,21 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="35" t="s">
-        <v>112</v>
+      <c r="C33" s="27" t="s">
+        <v>110</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37" t="s">
-        <v>116</v>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29" t="s">
+        <v>114</v>
       </c>
-      <c r="F33" s="38" t="s">
-        <v>117</v>
+      <c r="F33" s="30" t="s">
+        <v>115</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -2906,14 +2883,14 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="55" t="s">
-        <v>118</v>
+      <c r="A36" s="44" t="s">
+        <v>116</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2936,18 +2913,18 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="41" t="s">
-        <v>119</v>
+      <c r="B37" s="33" t="s">
+        <v>117</v>
       </c>
-      <c r="C37" s="58" t="s">
-        <v>120</v>
+      <c r="C37" s="47" t="s">
+        <v>118</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -2970,18 +2947,18 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
-        <v>121</v>
+      <c r="A38" s="12" t="s">
+        <v>119</v>
       </c>
-      <c r="B38" s="43">
+      <c r="B38" s="35">
         <v>10</v>
       </c>
-      <c r="C38" s="50" t="s">
-        <v>122</v>
+      <c r="C38" s="49" t="s">
+        <v>120</v>
       </c>
-      <c r="D38" s="49"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -3004,16 +2981,16 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
-        <v>123</v>
+      <c r="A39" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="B39" s="43" t="s">
-        <v>124</v>
+      <c r="B39" s="35" t="s">
+        <v>122</v>
       </c>
-      <c r="C39" s="50"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -3036,16 +3013,16 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21" t="s">
-        <v>125</v>
+      <c r="A40" s="19" t="s">
+        <v>123</v>
       </c>
-      <c r="B40" s="45">
+      <c r="B40" s="37">
         <v>3</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -3068,16 +3045,16 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="21" t="s">
-        <v>126</v>
+      <c r="A41" s="19" t="s">
+        <v>124</v>
       </c>
-      <c r="B41" s="45">
+      <c r="B41" s="37">
         <v>8</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -3100,16 +3077,16 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21" t="s">
-        <v>127</v>
+      <c r="A42" s="19" t="s">
+        <v>125</v>
       </c>
-      <c r="B42" s="45" t="s">
-        <v>124</v>
+      <c r="B42" s="37" t="s">
+        <v>122</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -3132,16 +3109,16 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="21" t="s">
-        <v>128</v>
+      <c r="A43" s="19" t="s">
+        <v>126</v>
       </c>
-      <c r="B43" s="45" t="s">
-        <v>124</v>
+      <c r="B43" s="37" t="s">
+        <v>122</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -3164,16 +3141,16 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21" t="s">
-        <v>129</v>
+      <c r="A44" s="19" t="s">
+        <v>127</v>
       </c>
-      <c r="B44" s="45" t="s">
-        <v>124</v>
+      <c r="B44" s="37" t="s">
+        <v>122</v>
       </c>
-      <c r="C44" s="48"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3196,16 +3173,16 @@
       <c r="Z44" s="3"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21" t="s">
-        <v>130</v>
+      <c r="A45" s="19" t="s">
+        <v>128</v>
       </c>
-      <c r="B45" s="45">
+      <c r="B45" s="37">
         <v>1</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3228,18 +3205,18 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21" t="s">
-        <v>131</v>
+      <c r="A46" s="19" t="s">
+        <v>129</v>
       </c>
-      <c r="B46" s="45">
+      <c r="B46" s="37">
         <v>1</v>
       </c>
-      <c r="C46" s="50" t="s">
-        <v>132</v>
+      <c r="C46" s="49" t="s">
+        <v>130</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3262,18 +3239,18 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22" t="s">
-        <v>133</v>
+      <c r="A47" s="20" t="s">
+        <v>131</v>
       </c>
-      <c r="B47" s="46" t="s">
-        <v>124</v>
+      <c r="B47" s="38" t="s">
+        <v>122</v>
       </c>
-      <c r="C47" s="51" t="s">
-        <v>132</v>
+      <c r="C47" s="40" t="s">
+        <v>130</v>
       </c>
-      <c r="D47" s="52"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -29980,13 +29957,6 @@
       <c r="Z1000" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:D33" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Digital Input"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="13">
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="H3:I3"/>
@@ -30021,68 +29991,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="4" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="5" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+    <row r="6" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+    <row r="7" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+    <row r="8" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+    <row r="9" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+    <row r="10" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+    <row r="11" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+    <row r="12" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+    <row r="13" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>